<commit_message>
Added automatic loading of tests from excel, with the results in excel
</commit_message>
<xml_diff>
--- a/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/DuplicateDatalocks.xlsx
+++ b/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/DuplicateDatalocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\das-providerpayments\src\PeriodEnd\PaymentsDue\SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests\ScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7B397621-CC98-4083-AFC6-3D2637BB928E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9E163CE2-5B90-44B9-A85D-9A1771768429}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223" activeTab="3" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223" firstSheet="1" activeTab="6" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
   </bookViews>
   <sheets>
     <sheet name="PastPayments" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Datalocks" sheetId="4" r:id="rId4"/>
     <sheet name="DatalockValidationErrors" sheetId="6" r:id="rId5"/>
     <sheet name="Commitments" sheetId="5" r:id="rId6"/>
+    <sheet name="Payments" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
   <si>
     <t>CommitmentId</t>
   </si>
@@ -177,6 +178,21 @@
   </si>
   <si>
     <t>TransactionTypesFlag</t>
+  </si>
+  <si>
+    <t>LearnRefNumber</t>
+  </si>
+  <si>
+    <t>learner a</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Transaction Type</t>
+  </si>
+  <si>
+    <t>Price Episode Identifier</t>
   </si>
 </sst>
 </file>
@@ -723,10 +739,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29113545-4422-48BA-A59E-5EDA0DBD892B}">
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection sqref="A1:AB11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -746,7 +762,7 @@
     <col min="28" max="28" width="26.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -831,8 +847,11 @@
       <c r="AB1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="AC1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -858,7 +877,7 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J2" t="s">
         <v>45</v>
@@ -917,8 +936,11 @@
       <c r="AB2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="AC2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -929,7 +951,7 @@
         <v>42979</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -944,7 +966,7 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J3" t="s">
         <v>45</v>
@@ -956,7 +978,7 @@
         <v>42979</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1003,8 +1025,11 @@
       <c r="AB3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="AC3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1015,7 +1040,7 @@
         <v>42979</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -1089,623 +1114,44 @@
       <c r="AB4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="2">
-        <v>42979</v>
-      </c>
-      <c r="C5" s="2">
-        <v>42979</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>25</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>23</v>
-      </c>
-      <c r="I5">
-        <v>0.9</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="2">
-        <v>42979</v>
-      </c>
-      <c r="M5">
-        <v>500</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="2">
-        <v>42979</v>
-      </c>
-      <c r="C6" s="2">
-        <v>42979</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>23</v>
-      </c>
-      <c r="I6">
-        <v>0.9</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="2">
-        <v>42979</v>
-      </c>
-      <c r="M6">
-        <v>500</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="2">
-        <v>43313</v>
-      </c>
-      <c r="C7" s="2">
-        <v>42979</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>25</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>23</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="2">
-        <v>42979</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="2">
-        <v>42979</v>
-      </c>
-      <c r="C8" s="2">
-        <v>42979</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>25</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>23</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="2">
-        <v>42979</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="2">
-        <v>42979</v>
-      </c>
-      <c r="C9" s="2">
-        <v>42979</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>25</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>23</v>
-      </c>
-      <c r="I9">
-        <v>0.9</v>
-      </c>
-      <c r="J9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="2">
-        <v>42979</v>
-      </c>
-      <c r="M9">
-        <v>1000</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="2">
-        <v>42979</v>
-      </c>
-      <c r="C10" s="2">
-        <v>42979</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>25</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>23</v>
-      </c>
-      <c r="I10">
-        <v>0.9</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="2">
-        <v>42979</v>
-      </c>
-      <c r="M10">
-        <v>1000</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
-      <c r="AB10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="2">
-        <v>42979</v>
-      </c>
-      <c r="C11" s="2">
-        <v>42979</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>25</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>23</v>
-      </c>
-      <c r="I11">
-        <v>0.9</v>
-      </c>
-      <c r="J11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="2">
-        <v>42979</v>
-      </c>
-      <c r="M11">
-        <v>1000</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="AC4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1832,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFDF27E-9B7C-47AE-A86A-FAE84BC024A3}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2544,4 +1990,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D57DEC8-9CE7-4F20-AF14-415D37453E52}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="17.07421875" customWidth="1"/>
+    <col min="2" max="2" width="11.53515625" customWidth="1"/>
+    <col min="3" max="3" width="20.53515625" customWidth="1"/>
+    <col min="4" max="4" width="21.765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added first day of academic year to payment calculations - essential to get the correct price episode identifier for Math/English that are paid in an academic year without onprog payments
</commit_message>
<xml_diff>
--- a/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/DuplicateDatalocks.xlsx
+++ b/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/DuplicateDatalocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\das-providerpayments\src\PeriodEnd\PaymentsDue\SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests\ScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9E163CE2-5B90-44B9-A85D-9A1771768429}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{332CC3D1-82D9-46B7-A0EB-85D3AC7383CE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223" firstSheet="1" activeTab="6" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="56">
   <si>
     <t>CommitmentId</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Price Episode Identifier</t>
+  </si>
+  <si>
+    <t>Delivery Year</t>
+  </si>
+  <si>
+    <t>Delivery Month</t>
   </si>
 </sst>
 </file>
@@ -1994,45 +2000,51 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D57DEC8-9CE7-4F20-AF14-415D37453E52}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.07421875" customWidth="1"/>
-    <col min="2" max="2" width="11.53515625" customWidth="1"/>
-    <col min="3" max="3" width="20.53515625" customWidth="1"/>
-    <col min="4" max="4" width="21.765625" customWidth="1"/>
+    <col min="1" max="2" width="17.07421875" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" customWidth="1"/>
+    <col min="4" max="4" width="20.53515625" customWidth="1"/>
+    <col min="5" max="5" width="21.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>2</v>
+        <v>2017</v>
       </c>
       <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
         <v>500</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>